<commit_message>
utolsó utolsó validálás, fixálás, etc
</commit_message>
<xml_diff>
--- a/kovetelmenyek.xlsx
+++ b/kovetelmenyek.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bence\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bence\Desktop\4th-semester\webterv\webterv-beadando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB601D8-8852-4D9B-BE93-C7E5ECD212AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F851C78C-CEA5-4AB5-8B13-E231050024BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="107">
   <si>
     <t>Részfeladat(ok)</t>
   </si>
@@ -249,98 +249,25 @@
     <t>style.css</t>
   </si>
   <si>
-    <t>10, 167</t>
-  </si>
-  <si>
     <t>login.html</t>
   </si>
   <si>
-    <t>23, 51</t>
-  </si>
-  <si>
-    <t>227, 342, 113</t>
-  </si>
-  <si>
     <t>260, 270</t>
   </si>
   <si>
-    <t>58, 73</t>
-  </si>
-  <si>
-    <t>etlap.html</t>
-  </si>
-  <si>
-    <t>292, 292, 186, 186</t>
-  </si>
-  <si>
-    <t>122, 16</t>
-  </si>
-  <si>
     <t>2, 14</t>
   </si>
   <si>
-    <t>347, 343</t>
-  </si>
-  <si>
-    <t>304, 108</t>
-  </si>
-  <si>
-    <t>128, 7, 403, 132</t>
-  </si>
-  <si>
     <t>134, 154, 133</t>
   </si>
   <si>
-    <t>422, 440</t>
-  </si>
-  <si>
-    <t>421, 119, 6</t>
-  </si>
-  <si>
-    <t>439, 418, 426, 314</t>
-  </si>
-  <si>
-    <t>437, 51</t>
-  </si>
-  <si>
     <t>17, 80</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Nem szabványosak az oldalak (Error: The character encoding was not declared. Proceeding using windows-1252.)</t>
   </si>
   <si>
-    <t>headers nincs!</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt; hiányzik</t>
-  </si>
-  <si>
-    <t>csak 4 féle űrlapelem van, 6 kellene; nincs alapállapot gomb</t>
-  </si>
-  <si>
-    <t>ez egy táblázat</t>
-  </si>
-  <si>
     <t>kész</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">50, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>93</t>
-    </r>
   </si>
   <si>
     <t>ez miért maradt ki a pontozásból?</t>
@@ -361,6 +288,186 @@
       <t>186</t>
     </r>
   </si>
+  <si>
+    <t>rolunk.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">headers nincs! // </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>kijavítva mindenhol</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">50, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>97</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ez egy táblázat // </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>kijavítva a megemlített helyen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2 // </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>hozzáadtam több beviteli mezőt labellel és mezőcsoportosítást</t>
+    </r>
+  </si>
+  <si>
+    <t>50, 95</t>
+  </si>
+  <si>
+    <t>10, 166</t>
+  </si>
+  <si>
+    <t>25, 53</t>
+  </si>
+  <si>
+    <t>227, 344, 113</t>
+  </si>
+  <si>
+    <t>60, 75</t>
+  </si>
+  <si>
+    <t>etlap.html / itallap.html</t>
+  </si>
+  <si>
+    <t>361, 361, 157, 157</t>
+  </si>
+  <si>
+    <t>124, 18</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a javított elemek sorszámát </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>piros</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>sal jelöltük</t>
+    </r>
+  </si>
+  <si>
+    <t>style.css / login.html</t>
+  </si>
+  <si>
+    <t>211 / 50</t>
+  </si>
+  <si>
+    <t>305, 108</t>
+  </si>
+  <si>
+    <t>348, 344</t>
+  </si>
+  <si>
+    <t>128, 7, 404, 132</t>
+  </si>
+  <si>
+    <t>423, 441</t>
+  </si>
+  <si>
+    <t>422, 6</t>
+  </si>
+  <si>
+    <t>440, 419, 427, 315</t>
+  </si>
+  <si>
+    <t>255, 264</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;strong&gt; hiányzik // </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>kijavítva a megemlített helyen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">csak 4 féle űrlapelem van, 6 kellene; nincs alapállapot gomb // </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>kijavítva a megemlített helyen</t>
+    </r>
+  </si>
+  <si>
+    <t>438, 51, 58</t>
+  </si>
 </sst>
 </file>
 
@@ -369,7 +476,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\.mm\.dd"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -453,6 +560,22 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -615,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,22 +884,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -997,10 +1123,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1100,10 +1226,10 @@
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="44" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="K3" s="43" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>9</v>
@@ -1138,7 +1264,7 @@
         <v>70</v>
       </c>
       <c r="J4" s="36">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="42">
         <v>1</v>
@@ -1174,7 +1300,7 @@
         <v>70</v>
       </c>
       <c r="J5" s="36">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K5" s="42">
         <v>1</v>
@@ -1208,7 +1334,7 @@
         <v>71</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="K6" s="42">
         <v>4</v>
@@ -1248,7 +1374,7 @@
         <v>70</v>
       </c>
       <c r="J7" s="36">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K7" s="42">
         <v>3</v>
@@ -1282,10 +1408,10 @@
         <v>70</v>
       </c>
       <c r="J8" s="36">
-        <v>124</v>
-      </c>
-      <c r="K8" s="42" t="s">
-        <v>93</v>
+        <v>126</v>
+      </c>
+      <c r="K8" s="43" t="s">
+        <v>82</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -1307,13 +1433,13 @@
       </c>
       <c r="H9" s="28"/>
       <c r="I9" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K9" s="43" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -1338,7 +1464,7 @@
         <v>70</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="K10" s="42">
         <v>1</v>
@@ -1370,7 +1496,7 @@
         <v>71</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="K11" s="42">
         <v>4</v>
@@ -1398,7 +1524,7 @@
         <v>71</v>
       </c>
       <c r="J12" s="36">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="K12" s="42">
         <v>2</v>
@@ -1422,14 +1548,14 @@
       <c r="H13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="37" t="s">
-        <v>71</v>
+      <c r="I13" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="J13" s="44">
         <v>116</v>
       </c>
       <c r="K13" s="43" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -1459,13 +1585,13 @@
         <v>6</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" s="36">
-        <v>58</v>
-      </c>
-      <c r="K14" s="42">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>85</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -1476,10 +1602,10 @@
       <c r="B15" s="47">
         <v>5</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="58" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="20" t="s">
@@ -1496,7 +1622,7 @@
         <v>71</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K15" s="42">
         <v>2</v>
@@ -1508,7 +1634,7 @@
     <row r="16" spans="1:14" ht="12.75">
       <c r="A16" s="48"/>
       <c r="B16" s="48"/>
-      <c r="C16" s="56"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="52"/>
       <c r="E16" s="20" t="s">
         <v>32</v>
@@ -1527,7 +1653,7 @@
     <row r="17" spans="1:14" ht="12.75">
       <c r="A17" s="48"/>
       <c r="B17" s="48"/>
-      <c r="C17" s="56"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="52"/>
       <c r="E17" s="20" t="s">
         <v>33</v>
@@ -1546,7 +1672,7 @@
     <row r="18" spans="1:14" ht="12.75">
       <c r="A18" s="48"/>
       <c r="B18" s="48"/>
-      <c r="C18" s="56"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="52"/>
       <c r="E18" s="20" t="s">
         <v>34</v>
@@ -1562,7 +1688,7 @@
         <v>70</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="K18" s="42">
         <v>1</v>
@@ -1574,7 +1700,7 @@
     <row r="19" spans="1:14" ht="12.75">
       <c r="A19" s="48"/>
       <c r="B19" s="48"/>
-      <c r="C19" s="56"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="52"/>
       <c r="E19" s="20" t="s">
         <v>35</v>
@@ -1593,7 +1719,7 @@
     <row r="20" spans="1:14" ht="12.75">
       <c r="A20" s="48"/>
       <c r="B20" s="48"/>
-      <c r="C20" s="56"/>
+      <c r="C20" s="60"/>
       <c r="D20" s="52"/>
       <c r="E20" s="20" t="s">
         <v>36</v>
@@ -1612,7 +1738,7 @@
     <row r="21" spans="1:14" ht="12.75">
       <c r="A21" s="48"/>
       <c r="B21" s="48"/>
-      <c r="C21" s="56"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="52"/>
       <c r="E21" s="20" t="s">
         <v>37</v>
@@ -1628,7 +1754,7 @@
         <v>70</v>
       </c>
       <c r="J21" s="36">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K21" s="42">
         <v>1</v>
@@ -1640,7 +1766,7 @@
     <row r="22" spans="1:14" ht="12.75">
       <c r="A22" s="48"/>
       <c r="B22" s="48"/>
-      <c r="C22" s="56"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="52"/>
       <c r="E22" s="20" t="s">
         <v>38</v>
@@ -1659,7 +1785,7 @@
     <row r="23" spans="1:14" ht="12.75">
       <c r="A23" s="48"/>
       <c r="B23" s="48"/>
-      <c r="C23" s="56"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="52"/>
       <c r="E23" s="20" t="s">
         <v>39</v>
@@ -1672,10 +1798,10 @@
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="37" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="K23" s="42">
         <v>4</v>
@@ -1687,7 +1813,7 @@
     <row r="24" spans="1:14" ht="12.75">
       <c r="A24" s="48"/>
       <c r="B24" s="48"/>
-      <c r="C24" s="56"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="52"/>
       <c r="E24" s="20" t="s">
         <v>40</v>
@@ -1703,7 +1829,7 @@
         <v>70</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="K24" s="42">
         <v>2</v>
@@ -1715,8 +1841,8 @@
     <row r="25" spans="1:14" ht="12.75">
       <c r="A25" s="48"/>
       <c r="B25" s="48"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="60" t="s">
+      <c r="C25" s="60"/>
+      <c r="D25" s="58" t="s">
         <v>41</v>
       </c>
       <c r="E25" s="20" t="s">
@@ -1736,7 +1862,7 @@
     <row r="26" spans="1:14" ht="12.75">
       <c r="A26" s="48"/>
       <c r="B26" s="48"/>
-      <c r="C26" s="56"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="52"/>
       <c r="E26" s="20" t="s">
         <v>43</v>
@@ -1752,7 +1878,7 @@
         <v>71</v>
       </c>
       <c r="J26" s="36" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K26" s="42">
         <v>1</v>
@@ -1764,7 +1890,7 @@
     <row r="27" spans="1:14" ht="12.75">
       <c r="A27" s="48"/>
       <c r="B27" s="48"/>
-      <c r="C27" s="56"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="52"/>
       <c r="E27" s="20" t="s">
         <v>44</v>
@@ -1783,7 +1909,7 @@
     <row r="28" spans="1:14" ht="12.75">
       <c r="A28" s="48"/>
       <c r="B28" s="48"/>
-      <c r="C28" s="56"/>
+      <c r="C28" s="60"/>
       <c r="D28" s="52"/>
       <c r="E28" s="20" t="s">
         <v>45</v>
@@ -1796,10 +1922,10 @@
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="J28" s="36">
-        <v>210</v>
+        <v>95</v>
+      </c>
+      <c r="J28" s="36" t="s">
+        <v>96</v>
       </c>
       <c r="K28" s="42">
         <v>1</v>
@@ -1811,7 +1937,7 @@
     <row r="29" spans="1:14" ht="12.75">
       <c r="A29" s="48"/>
       <c r="B29" s="48"/>
-      <c r="C29" s="56"/>
+      <c r="C29" s="60"/>
       <c r="D29" s="52"/>
       <c r="E29" s="20" t="s">
         <v>46</v>
@@ -1827,7 +1953,7 @@
         <v>71</v>
       </c>
       <c r="J29" s="36" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="K29" s="42">
         <v>1</v>
@@ -1839,7 +1965,7 @@
     <row r="30" spans="1:14" ht="12.75">
       <c r="A30" s="48"/>
       <c r="B30" s="48"/>
-      <c r="C30" s="56"/>
+      <c r="C30" s="60"/>
       <c r="D30" s="52"/>
       <c r="E30" s="20" t="s">
         <v>47</v>
@@ -1855,7 +1981,7 @@
         <v>71</v>
       </c>
       <c r="J30" s="36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="K30" s="42">
         <v>1</v>
@@ -1867,7 +1993,7 @@
     <row r="31" spans="1:14" ht="12.75">
       <c r="A31" s="48"/>
       <c r="B31" s="48"/>
-      <c r="C31" s="56"/>
+      <c r="C31" s="60"/>
       <c r="D31" s="52"/>
       <c r="E31" s="20" t="s">
         <v>48</v>
@@ -1880,24 +2006,22 @@
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="J31" s="36">
-        <v>122</v>
-      </c>
-      <c r="K31" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="L31" s="39" t="s">
-        <v>91</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="J31" s="44">
+        <v>80</v>
+      </c>
+      <c r="K31" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" s="39"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" ht="30.75" customHeight="1">
       <c r="A32" s="48"/>
       <c r="B32" s="48"/>
-      <c r="C32" s="56"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="52"/>
       <c r="E32" s="32" t="s">
         <v>49</v>
@@ -1913,7 +2037,7 @@
         <v>71</v>
       </c>
       <c r="J32" s="36" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="K32" s="42">
         <v>4</v>
@@ -1925,7 +2049,7 @@
     <row r="33" spans="1:14" ht="12.75">
       <c r="A33" s="48"/>
       <c r="B33" s="48"/>
-      <c r="C33" s="56"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="52"/>
       <c r="E33" s="20" t="s">
         <v>50</v>
@@ -1941,7 +2065,7 @@
         <v>71</v>
       </c>
       <c r="J33" s="36" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="K33" s="42">
         <v>1</v>
@@ -1953,7 +2077,7 @@
     <row r="34" spans="1:14" ht="12.75">
       <c r="A34" s="48"/>
       <c r="B34" s="48"/>
-      <c r="C34" s="56"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="52"/>
       <c r="E34" s="39" t="s">
         <v>51</v>
@@ -1969,7 +2093,7 @@
         <v>71</v>
       </c>
       <c r="J34" s="36" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -1978,7 +2102,7 @@
     <row r="35" spans="1:14" ht="12.75">
       <c r="A35" s="48"/>
       <c r="B35" s="48"/>
-      <c r="C35" s="56"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="52"/>
       <c r="E35" s="20" t="s">
         <v>52</v>
@@ -1997,7 +2121,7 @@
     <row r="36" spans="1:14" ht="12.75">
       <c r="A36" s="48"/>
       <c r="B36" s="48"/>
-      <c r="C36" s="56"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="52"/>
       <c r="E36" s="20" t="s">
         <v>53</v>
@@ -2013,7 +2137,7 @@
         <v>71</v>
       </c>
       <c r="J36" s="36">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="K36" s="42">
         <v>2</v>
@@ -2025,7 +2149,7 @@
     <row r="37" spans="1:14" ht="12.75">
       <c r="A37" s="48"/>
       <c r="B37" s="48"/>
-      <c r="C37" s="56"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="52"/>
       <c r="E37" s="20" t="s">
         <v>54</v>
@@ -2044,7 +2168,7 @@
     <row r="38" spans="1:14" ht="12.75">
       <c r="A38" s="48"/>
       <c r="B38" s="48"/>
-      <c r="C38" s="56"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="52"/>
       <c r="E38" s="20" t="s">
         <v>55</v>
@@ -2060,7 +2184,7 @@
         <v>71</v>
       </c>
       <c r="J38" s="36" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="K38" s="42">
         <v>1</v>
@@ -2072,7 +2196,7 @@
     <row r="39" spans="1:14" ht="12.75">
       <c r="A39" s="48"/>
       <c r="B39" s="48"/>
-      <c r="C39" s="56"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="52"/>
       <c r="E39" s="20" t="s">
         <v>56</v>
@@ -2088,7 +2212,7 @@
         <v>71</v>
       </c>
       <c r="J39" s="36" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="K39" s="42">
         <v>2</v>
@@ -2100,7 +2224,7 @@
     <row r="40" spans="1:14" ht="12.75">
       <c r="A40" s="48"/>
       <c r="B40" s="48"/>
-      <c r="C40" s="56"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="52"/>
       <c r="E40" s="39" t="s">
         <v>67</v>
@@ -2117,8 +2241,8 @@
     <row r="41" spans="1:14" ht="12.75">
       <c r="A41" s="48"/>
       <c r="B41" s="48"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="60" t="s">
+      <c r="C41" s="60"/>
+      <c r="D41" s="58" t="s">
         <v>57</v>
       </c>
       <c r="E41" s="20" t="s">
@@ -2135,21 +2259,19 @@
         <v>71</v>
       </c>
       <c r="J41" s="36" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="K41" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="L41" s="39" t="s">
-        <v>91</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="L41" s="39"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:14" ht="12.75">
       <c r="A42" s="48"/>
       <c r="B42" s="48"/>
-      <c r="C42" s="56"/>
+      <c r="C42" s="60"/>
       <c r="D42" s="52"/>
       <c r="E42" s="20" t="s">
         <v>59</v>
@@ -2164,19 +2286,20 @@
       <c r="I42" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="J42" s="36">
-        <v>252</v>
-      </c>
-      <c r="L42" s="39" t="s">
-        <v>91</v>
-      </c>
+      <c r="J42" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="K42" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="L42" s="39"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="1:14" ht="12.75">
       <c r="A43" s="48"/>
       <c r="B43" s="48"/>
-      <c r="C43" s="56"/>
+      <c r="C43" s="60"/>
       <c r="D43" s="52"/>
       <c r="E43" s="20" t="s">
         <v>60</v>
@@ -2195,7 +2318,7 @@
     <row r="44" spans="1:14" ht="12.75">
       <c r="A44" s="48"/>
       <c r="B44" s="48"/>
-      <c r="C44" s="56"/>
+      <c r="C44" s="60"/>
       <c r="D44" s="52"/>
       <c r="E44" s="20" t="s">
         <v>61</v>
@@ -2211,7 +2334,7 @@
         <v>71</v>
       </c>
       <c r="J44" s="36" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="K44" s="42">
         <v>2</v>
@@ -2223,7 +2346,7 @@
     <row r="45" spans="1:14" ht="12.75">
       <c r="A45" s="48"/>
       <c r="B45" s="48"/>
-      <c r="C45" s="56"/>
+      <c r="C45" s="60"/>
       <c r="D45" s="52"/>
       <c r="E45" s="20" t="s">
         <v>62</v>
@@ -2239,7 +2362,7 @@
         <v>71</v>
       </c>
       <c r="J45" s="36" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="K45" s="42">
         <v>2</v>
@@ -2251,7 +2374,7 @@
     <row r="46" spans="1:14" ht="12.75">
       <c r="A46" s="48"/>
       <c r="B46" s="48"/>
-      <c r="C46" s="56"/>
+      <c r="C46" s="60"/>
       <c r="D46" s="52"/>
       <c r="E46" s="20" t="s">
         <v>63</v>
@@ -2267,7 +2390,7 @@
         <v>71</v>
       </c>
       <c r="J46" s="36">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K46" s="42">
         <v>2</v>
@@ -2279,7 +2402,7 @@
     <row r="47" spans="1:14" ht="12.75">
       <c r="A47" s="48"/>
       <c r="B47" s="48"/>
-      <c r="C47" s="56"/>
+      <c r="C47" s="60"/>
       <c r="D47" s="52"/>
       <c r="E47" s="20" t="s">
         <v>64</v>
@@ -2298,7 +2421,7 @@
     <row r="48" spans="1:14" ht="12.75" customHeight="1">
       <c r="A48" s="48"/>
       <c r="B48" s="48"/>
-      <c r="C48" s="56"/>
+      <c r="C48" s="60"/>
       <c r="D48" s="52"/>
       <c r="E48" s="20" t="s">
         <v>65</v>
@@ -2309,7 +2432,7 @@
       <c r="G48" s="10"/>
       <c r="H48" s="41"/>
       <c r="I48" s="37"/>
-      <c r="J48" s="57"/>
+      <c r="J48" s="55"/>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
@@ -2317,7 +2440,7 @@
     <row r="49" spans="1:14" ht="12.75">
       <c r="A49" s="48"/>
       <c r="B49" s="48"/>
-      <c r="C49" s="56"/>
+      <c r="C49" s="60"/>
       <c r="D49" s="52"/>
       <c r="E49" s="20" t="s">
         <v>66</v>
@@ -2328,7 +2451,7 @@
       <c r="G49" s="10"/>
       <c r="H49" s="28"/>
       <c r="I49" s="31"/>
-      <c r="J49" s="58"/>
+      <c r="J49" s="56"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
@@ -2336,7 +2459,7 @@
     <row r="50" spans="1:14" ht="12.75">
       <c r="A50" s="48"/>
       <c r="B50" s="48"/>
-      <c r="C50" s="56"/>
+      <c r="C50" s="60"/>
       <c r="D50" s="52"/>
       <c r="E50" s="20" t="s">
         <v>67</v>
@@ -2345,7 +2468,7 @@
       <c r="G50" s="10"/>
       <c r="H50" s="28"/>
       <c r="I50" s="31"/>
-      <c r="J50" s="59"/>
+      <c r="J50" s="57"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
@@ -2361,18 +2484,26 @@
       <c r="H51" s="25"/>
       <c r="I51" s="25"/>
       <c r="J51" s="22"/>
+      <c r="K51" s="61" t="s">
+        <v>94</v>
+      </c>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
     </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1">
+      <c r="K52" s="61"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="K51:K52"/>
     <mergeCell ref="J48:J50"/>
     <mergeCell ref="D15:D24"/>
     <mergeCell ref="D25:D40"/>
     <mergeCell ref="D41:D50"/>
     <mergeCell ref="A14:A50"/>
     <mergeCell ref="B15:B50"/>
+    <mergeCell ref="C15:C50"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="C2:D2"/>
@@ -2383,7 +2514,6 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C15:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>